<commit_message>
28.07.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Requisition/July/28.07.2020 Requisition of Mugdho Corporation.xlsx
+++ b/2020/Requisition/July/28.07.2020 Requisition of Mugdho Corporation.xlsx
@@ -1105,7 +1105,7 @@
       <pane xSplit="4" ySplit="15" topLeftCell="E16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="J124" sqref="J124"/>
+      <selection pane="bottomRight" activeCell="G119" sqref="G119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -5379,7 +5379,7 @@
         <v>21</v>
       </c>
       <c r="C116" s="15">
-        <v>800000</v>
+        <v>700000</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>136</v>
@@ -5538,7 +5538,7 @@
       </c>
       <c r="C120" s="16">
         <f>SUBTOTAL(9,C115:C119)</f>
-        <v>800000</v>
+        <v>700000</v>
       </c>
       <c r="D120" s="11"/>
       <c r="E120" s="17"/>

</xml_diff>